<commit_message>
Ajuste esqueleto de guion falta
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="2772" windowWidth="15108" windowHeight="5964" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="108" yWindow="2772" windowWidth="15108" windowHeight="5964" tabRatio="729" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,7 @@
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -91,9 +84,6 @@
     <t>MA_07_01_CO</t>
   </si>
   <si>
-    <t>Educación secundaria obligatoria</t>
-  </si>
-  <si>
     <t>Matemáticas</t>
   </si>
   <si>
@@ -239,6 +229,9 @@
   </si>
   <si>
     <t>MA_07_01</t>
+  </si>
+  <si>
+    <t>Educación Básica Secundaria</t>
   </si>
 </sst>
 </file>
@@ -1295,14 +1288,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1572,7 +1557,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1602,7 +1587,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1610,7 +1595,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1626,17 +1611,12 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1644,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1682,19 +1662,19 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="15.6">
       <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>26</v>
-      </c>
       <c r="E2" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="16">
         <v>3</v>
@@ -1708,19 +1688,19 @@
     </row>
     <row r="3" spans="1:12" ht="15.6">
       <c r="A3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="16">
         <v>4</v>
@@ -1728,19 +1708,19 @@
     </row>
     <row r="4" spans="1:12" ht="15.6">
       <c r="A4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="16">
         <v>5</v>
@@ -1748,19 +1728,19 @@
     </row>
     <row r="5" spans="1:12" ht="15.6">
       <c r="A5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="39">
         <v>7</v>
@@ -1768,19 +1748,19 @@
     </row>
     <row r="6" spans="1:12" ht="15.6">
       <c r="A6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="39">
         <v>8</v>
@@ -1788,19 +1768,19 @@
     </row>
     <row r="7" spans="1:12" ht="15.6">
       <c r="A7" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="39">
         <v>10</v>
@@ -1808,19 +1788,19 @@
     </row>
     <row r="8" spans="1:12" ht="15.6">
       <c r="A8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="39">
         <v>11</v>
@@ -1828,19 +1808,19 @@
     </row>
     <row r="9" spans="1:12" ht="15.6">
       <c r="A9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="39">
         <v>12</v>
@@ -1849,19 +1829,19 @@
     </row>
     <row r="10" spans="1:12" ht="15.6">
       <c r="A10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="39">
         <v>13</v>
@@ -1870,19 +1850,19 @@
     </row>
     <row r="11" spans="1:12" ht="15.6">
       <c r="A11" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="39">
         <v>14</v>
@@ -1891,19 +1871,19 @@
     </row>
     <row r="12" spans="1:12" ht="15.6">
       <c r="A12" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="39" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="39">
         <v>15</v>
@@ -1912,19 +1892,19 @@
     </row>
     <row r="13" spans="1:12" ht="15.6">
       <c r="A13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="C13" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="14">
         <v>17</v>
@@ -1932,19 +1912,19 @@
     </row>
     <row r="14" spans="1:12" ht="15.6">
       <c r="A14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="14">
         <v>18</v>
@@ -1953,11 +1933,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1966,12 +1941,12 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="66.109375" customWidth="1"/>
+    <col min="1" max="1" width="76.44140625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1988,10 +1963,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
@@ -1999,10 +1974,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -2010,10 +1985,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1">
       <c r="A4" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="19">
         <v>6</v>
@@ -2021,10 +1996,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1">
       <c r="A5" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="37">
         <v>9</v>
@@ -2032,10 +2007,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="37">
         <v>16</v>
@@ -2043,10 +2018,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="30">
         <v>19</v>
@@ -2054,10 +2029,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="30">
         <v>20</v>
@@ -2069,11 +2044,6 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2084,7 +2054,7 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2111,10 +2081,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2122,10 +2092,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2133,10 +2103,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2144,10 +2114,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2155,10 +2125,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2166,10 +2136,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2177,10 +2147,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2188,10 +2158,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2199,10 +2169,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2210,10 +2180,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2221,10 +2191,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2232,10 +2202,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2243,10 +2213,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2254,10 +2224,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2265,10 +2235,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2276,10 +2246,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2287,10 +2257,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2298,10 +2268,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2309,10 +2279,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2320,10 +2290,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="3:3">
@@ -2336,11 +2306,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2399,10 +2364,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2416,14 +2381,14 @@
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -2435,14 +2400,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -2454,14 +2419,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2473,14 +2438,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2492,14 +2457,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -2511,14 +2476,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2530,14 +2495,14 @@
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -2549,14 +2514,14 @@
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2568,14 +2533,14 @@
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2587,14 +2552,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -2606,14 +2571,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -2625,14 +2590,14 @@
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
@@ -2644,14 +2609,14 @@
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -2663,14 +2628,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2682,14 +2647,14 @@
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2701,22 +2666,22 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2724,14 +2689,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2743,22 +2708,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2766,10 +2731,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2783,10 +2748,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2800,10 +2765,10 @@
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -2817,20 +2782,20 @@
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2838,20 +2803,20 @@
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2859,20 +2824,20 @@
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2880,14 +2845,14 @@
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -2899,22 +2864,22 @@
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2922,10 +2887,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -2939,20 +2904,20 @@
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2960,14 +2925,14 @@
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -2979,22 +2944,22 @@
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3002,18 +2967,18 @@
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
@@ -3023,18 +2988,18 @@
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
@@ -3044,18 +3009,18 @@
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H35" s="23"/>
       <c r="I35" s="23"/>
@@ -3065,18 +3030,18 @@
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -3086,18 +3051,18 @@
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -3107,24 +3072,24 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3132,18 +3097,18 @@
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -3153,18 +3118,18 @@
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -3174,18 +3139,18 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
@@ -3195,18 +3160,18 @@
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
@@ -3216,24 +3181,24 @@
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3241,24 +3206,24 @@
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3266,24 +3231,24 @@
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3291,14 +3256,14 @@
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
@@ -3310,22 +3275,22 @@
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
       <c r="H47" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3333,22 +3298,22 @@
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
       <c r="H48" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3356,22 +3321,22 @@
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3379,14 +3344,14 @@
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
@@ -3398,22 +3363,22 @@
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
       <c r="H51" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3421,20 +3386,20 @@
         <v>19</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
       <c r="H52" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3442,20 +3407,20 @@
         <v>19</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3463,10 +3428,10 @@
         <v>19</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D54" s="31"/>
       <c r="E54" s="31"/>
@@ -3480,20 +3445,20 @@
         <v>19</v>
       </c>
       <c r="B55" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="30" t="s">
         <v>67</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>68</v>
       </c>
       <c r="D55" s="31"/>
       <c r="E55" s="31"/>
       <c r="F55" s="31"/>
       <c r="G55" s="31"/>
       <c r="H55" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I55" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3514,10 +3479,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Esqueleto de guion ajustado
Se ajustó el esqueleto de guion según indicaciones de Oliver y Lizzie.
Se está ajustando el guion 01 de acuerdo a observaciones de Lizzie,
faltan los recursos de profundiza que debe agregar la autora para
completar el material.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="108" yWindow="2772" windowWidth="15108" windowHeight="5964" tabRatio="729" activeTab="3"/>
+    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,13 +18,12 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="72">
   <si>
     <t>FICHA</t>
   </si>
@@ -90,51 +94,18 @@
     <t>Los números enteros son un conjunto numérico que amplía el uso de los números en situaciones que no son posibles de describir con los números naturales.</t>
   </si>
   <si>
-    <t>1° ESO</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
-    <t>¿Mayor o menor?</t>
-  </si>
-  <si>
     <t>Ordena números enteros</t>
   </si>
   <si>
     <t>Ordena de menor a mayor números enteros</t>
   </si>
   <si>
-    <t>¿Para qué se usan los números enteros?</t>
-  </si>
-  <si>
-    <t>Sucesiones de números enteros</t>
-  </si>
-  <si>
-    <t>¿Qué sabes del valor absoluto y de los números opuestos?</t>
-  </si>
-  <si>
-    <t>Valor absoluto y números opuestos</t>
-  </si>
-  <si>
-    <t>El valor absoluto y el opuesto de un número entero</t>
-  </si>
-  <si>
-    <t>Analiza situaciones que requieren del uso de los números enteros</t>
-  </si>
-  <si>
     <t>¿Qué sabes de los números enteros?</t>
   </si>
   <si>
-    <t xml:space="preserve">Sustracciones que dan números enteros </t>
-  </si>
-  <si>
-    <t>Competencias: Justifico la elección de métodos e instrumentos de dominios numéricos, en la resolución de problemas.</t>
-  </si>
-  <si>
-    <t>Competencias: Identifica características de localización de objetos en sistemas de representación como rectas numéricas.</t>
-  </si>
-  <si>
     <t>¿Cómo hacer una recta numérica?</t>
   </si>
   <si>
@@ -216,9 +187,6 @@
     <t>La aplicación de los números enteros en la vida cotidiana</t>
   </si>
   <si>
-    <t>Ejercitación y competencias</t>
-  </si>
-  <si>
     <t>Fin de tema</t>
   </si>
   <si>
@@ -228,17 +196,56 @@
     <t>Refuerza tu aprendizaje: ubicación de números enteros y situaciones en las que se usan</t>
   </si>
   <si>
-    <t>MA_07_01</t>
-  </si>
-  <si>
     <t>Educación Básica Secundaria</t>
+  </si>
+  <si>
+    <t>2° ESO</t>
+  </si>
+  <si>
+    <t>Los números enteros</t>
+  </si>
+  <si>
+    <t>¿Mayor o menor en la recta?</t>
+  </si>
+  <si>
+    <t>MT_07_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lo esencial de los números enteros </t>
+  </si>
+  <si>
+    <t>Completa la serie de números de enteros</t>
+  </si>
+  <si>
+    <t>¿Qué sabes de valores absolutos y opuestos?</t>
+  </si>
+  <si>
+    <t>Encuentra la pareja de números enteros</t>
+  </si>
+  <si>
+    <t>El valor absoluto y opuesto de un número entero</t>
+  </si>
+  <si>
+    <t>Piensa en relación a los números enteros</t>
+  </si>
+  <si>
+    <t>¿Restas con resultado natural o entero?</t>
+  </si>
+  <si>
+    <t>Competencias: identifica frases con valores numéricos</t>
+  </si>
+  <si>
+    <t>Competencias: identifica fechas históricas</t>
+  </si>
+  <si>
+    <t>Competencias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,20 +294,6 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -802,7 +795,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -856,8 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -879,9 +870,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1288,6 +1276,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1546,27 +1542,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="136.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1574,7 +1570,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1590,15 +1586,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1606,7 +1602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1621,26 +1617,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1660,21 +1656,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="15.6">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="F2" s="16">
         <v>3</v>
@@ -1686,245 +1682,245 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.6">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>69</v>
+      <c r="E3" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="F3" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="C4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="F4" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="38" t="s">
+      <c r="C5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="23">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="23">
+        <v>13</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="23">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="23">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.6">
-      <c r="A6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F6" s="39">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.6">
-      <c r="A7" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.6">
-      <c r="A8" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="39">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.6">
-      <c r="A9" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="39">
-        <v>12</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.6">
-      <c r="A10" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="39">
-        <v>13</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.6">
-      <c r="A11" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="39">
-        <v>14</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.6">
-      <c r="A12" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="39">
-        <v>15</v>
-      </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.6">
-      <c r="A13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>69</v>
+      <c r="E13" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="F13" s="14">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.6">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="F14" s="14">
         <v>18</v>
@@ -1937,20 +1933,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="76.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1961,80 +1957,80 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C4" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
-      <c r="A5" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="37">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="35">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="37">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="35">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="30">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="30">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="28">
         <v>20</v>
       </c>
     </row>
@@ -2048,24 +2044,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2076,227 +2072,227 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>27</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="B13" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>13</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>14</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>32</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>17</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="B18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>18</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="30">
-        <v>19</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="30">
+      <c r="B19" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="28">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
         <v>20</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3">
+      <c r="B21" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
     </row>
   </sheetData>
@@ -2310,27 +2306,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="D27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.77734375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="71.5546875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="71.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2359,15 +2355,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2376,365 +2372,365 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2743,15 +2739,15 @@
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2760,15 +2756,15 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -2777,120 +2773,120 @@
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="16" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
       <c r="H25" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
       <c r="H26" s="16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="20" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="16" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -2899,581 +2895,581 @@
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="23" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="23" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H35" s="23"/>
       <c r="I35" s="23"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H43" s="21" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="H43" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="H44" s="21" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>66</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
       <c r="H47" s="23" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
       <c r="H48" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I49" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
       <c r="H51" s="23" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
       <c r="H52" s="14" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="14" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="C55" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="I55" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I55" s="29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes punto final títulos recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="100" yWindow="2780" windowWidth="15100" windowHeight="5980" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,12 +13,17 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="125725" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="71">
   <si>
     <t>FICHA</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: ubicación de números enteros y situaciones en las que se usan.</t>
   </si>
   <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: orden en el conjunto de los números enteros </t>
@@ -1542,7 +1539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1552,17 +1549,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" zoomScalePageLayoutView="235" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="136.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1570,7 +1567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1586,15 +1583,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1613,6 +1610,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1620,23 +1622,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1656,21 +1658,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1">
       <c r="A2" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="F2" s="16">
         <v>3</v>
@@ -1682,245 +1684,245 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="23">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="23">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="23">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="23">
         <v>12</v>
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="23">
         <v>13</v>
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="23">
         <v>14</v>
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="23">
         <v>15</v>
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="14">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="14">
         <v>18</v>
@@ -1928,7 +1930,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1936,17 +1943,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" zoomScalePageLayoutView="205" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="76.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="76.5" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1957,7 +1964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1">
       <c r="A2" s="15" t="s">
         <v>27</v>
       </c>
@@ -1968,9 +1975,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1">
       <c r="A3" s="15" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>28</v>
@@ -1979,9 +1986,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1">
       <c r="A4" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>28</v>
@@ -1990,9 +1997,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1">
       <c r="A5" s="35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>28</v>
@@ -2001,9 +2008,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>28</v>
@@ -2012,9 +2019,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>28</v>
@@ -2023,9 +2030,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>28</v>
@@ -2040,28 +2047,33 @@
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2072,7 +2084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2083,29 +2095,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2113,10 +2125,10 @@
         <v>24</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2124,98 +2136,98 @@
         <v>25</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="19">
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="21">
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="21">
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="21">
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="21">
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="21">
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="21">
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="21">
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -2223,76 +2235,76 @@
         <v>26</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="21">
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="21">
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="25">
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="25">
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="28">
         <v>19</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="28">
         <v>20</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3">
       <c r="C40" s="6"/>
     </row>
   </sheetData>
@@ -2302,6 +2314,11 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2309,24 +2326,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="71.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="70.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="71.5" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2355,15 +2372,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2372,304 +2389,304 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -2680,57 +2697,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I20" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -2739,15 +2756,15 @@
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
@@ -2756,15 +2773,15 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
@@ -2773,36 +2790,36 @@
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2812,18 +2829,18 @@
         <v>24</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -2833,60 +2850,60 @@
         <v>25</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="19" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -2895,413 +2912,413 @@
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I32" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="21"/>
       <c r="D33" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H33" s="23"/>
       <c r="I33" s="23"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H35" s="23"/>
       <c r="I35" s="23"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I38" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H41" s="23"/>
       <c r="I41" s="23"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H43" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H44" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I44" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H45" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
       <c r="H47" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
@@ -3309,125 +3326,125 @@
         <v>26</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
       <c r="H51" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I51" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
       <c r="H52" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29"/>
@@ -3436,44 +3453,49 @@
       <c r="H54" s="27"/>
       <c r="I54" s="27"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" s="28" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="28" t="s">
         <v>54</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>55</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29"/>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
       <c r="H55" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I55" s="29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MA0701: Ajustes previos a la carga en GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="106" yWindow="2774" windowWidth="15109" windowHeight="5971" tabRatio="729" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>La aplicación de los números enteros en la vida cotidiana</t>
   </si>
   <si>
-    <t>Fin de tema</t>
-  </si>
-  <si>
     <t>Evaluación</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Construcción de una recta numérica</t>
+  </si>
+  <si>
+    <t>Más información</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +363,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -804,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -858,11 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,6 +897,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1581,13 +1584,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="136.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="136.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1611,15 +1614,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1649,19 +1652,19 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1681,21 +1684,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="F2" s="16">
         <v>4</v>
@@ -1707,245 +1710,245 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="23">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="23">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="23">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="23">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="23">
         <v>13</v>
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="23">
         <v>14</v>
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F11" s="23">
         <v>15</v>
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="23">
         <v>16</v>
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="14">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="14">
         <v>19</v>
@@ -1965,13 +1968,13 @@
       <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="76.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="76.3984375" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1982,18 +1985,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="36" t="s">
+    <row r="2" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+      <c r="A2" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -2004,7 +2007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
         <v>30</v>
       </c>
@@ -2026,47 +2029,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="33">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="33">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="27">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>21</v>
       </c>
     </row>
@@ -2090,15 +2093,15 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2113,14 +2116,14 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37">
+    <row r="2" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="38" t="s">
+      <c r="B2" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="5"/>
@@ -2128,134 +2131,134 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="19">
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="19">
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="19">
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="19">
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="21">
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="21">
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="21">
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="5"/>
@@ -2263,14 +2266,14 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="21">
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="5"/>
@@ -2278,14 +2281,14 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="21">
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="5"/>
@@ -2293,14 +2296,14 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="21">
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="5"/>
@@ -2308,14 +2311,14 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="21">
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="5"/>
@@ -2323,14 +2326,14 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="21">
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="5"/>
@@ -2338,14 +2341,14 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="21">
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="5"/>
@@ -2353,14 +2356,14 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="21">
         <v>17</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="5"/>
@@ -2368,14 +2371,14 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="25">
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="31" t="s">
         <v>35</v>
       </c>
       <c r="E19" s="5"/>
@@ -2383,14 +2386,14 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="25">
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="5"/>
@@ -2398,14 +2401,14 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="27">
         <v>20</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="32" t="s">
         <v>28</v>
       </c>
       <c r="E21" s="5"/>
@@ -2413,14 +2416,14 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="27">
         <v>21</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="32" t="s">
         <v>28</v>
       </c>
       <c r="E22" s="5"/>
@@ -2428,31 +2431,31 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C41" s="6"/>
     </row>
   </sheetData>
@@ -2469,24 +2472,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:I58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="71.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.73046875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.73046875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.73046875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="71.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
@@ -2532,7 +2535,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -2551,7 +2554,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
@@ -2570,7 +2573,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
@@ -2589,7 +2592,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
@@ -2608,7 +2611,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2630,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -2646,7 +2649,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -2665,7 +2668,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
@@ -2684,7 +2687,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -2722,7 +2725,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -2741,7 +2744,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
@@ -2760,7 +2763,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
@@ -2779,7 +2782,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
@@ -2798,7 +2801,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>19</v>
       </c>
@@ -2817,7 +2820,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
@@ -2833,14 +2836,14 @@
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="36" t="s">
-        <v>72</v>
+      <c r="H18" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -2859,7 +2862,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
@@ -2878,7 +2881,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>19</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
@@ -2920,7 +2923,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="15" t="s">
         <v>19</v>
       </c>
@@ -2937,13 +2940,13 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
@@ -2960,7 +2963,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
@@ -2977,7 +2980,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
         <v>19</v>
       </c>
@@ -2994,7 +2997,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="19" t="s">
         <v>19</v>
       </c>
@@ -3009,13 +3012,13 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>19</v>
       </c>
@@ -3036,7 +3039,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="19" t="s">
         <v>19</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="19" t="s">
         <v>19</v>
       </c>
@@ -3076,7 +3079,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="19" t="s">
         <v>19</v>
       </c>
@@ -3099,7 +3102,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
@@ -3116,7 +3119,7 @@
       <c r="H32" s="23"/>
       <c r="I32" s="23"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
@@ -3131,13 +3134,13 @@
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I33" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
@@ -3156,7 +3159,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
@@ -3173,13 +3176,13 @@
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
@@ -3200,7 +3203,7 @@
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
@@ -3221,7 +3224,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
@@ -3242,7 +3245,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
@@ -3263,7 +3266,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
@@ -3284,7 +3287,7 @@
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
@@ -3330,7 +3333,7 @@
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
@@ -3351,7 +3354,7 @@
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
@@ -3372,7 +3375,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
@@ -3393,7 +3396,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
@@ -3412,13 +3415,13 @@
         <v>44</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I46" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
@@ -3437,13 +3440,13 @@
         <v>44</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I47" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
@@ -3462,13 +3465,13 @@
         <v>49</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I48" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
@@ -3487,7 +3490,7 @@
       <c r="H49" s="23"/>
       <c r="I49" s="23"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
@@ -3504,13 +3507,13 @@
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I50" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
@@ -3550,13 +3553,13 @@
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I52" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
@@ -3575,7 +3578,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
@@ -3598,12 +3601,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C55" s="25" t="s">
         <v>49</v>
@@ -3613,18 +3616,18 @@
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
       <c r="H55" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I55" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="25" t="s">
         <v>49</v>
@@ -3634,65 +3637,65 @@
       <c r="F56" s="26"/>
       <c r="G56" s="26"/>
       <c r="H56" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I56" s="26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="28" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A58" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27" t="s">
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I58" s="40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I58" s="29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MA0701: Ajuste de errores de Esqueleto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="106" yWindow="2774" windowWidth="15109" windowHeight="5971" tabRatio="729" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="106" yWindow="2774" windowWidth="15109" windowHeight="5971" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="71">
   <si>
     <t>FICHA</t>
   </si>
@@ -112,9 +112,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: ubicación de números enteros y situaciones en las que se usan.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Refuerza tu aprendizaje: orden en el conjunto de los números enteros </t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>Mapa conceptual</t>
-  </si>
-  <si>
-    <t>Autoevaluación</t>
   </si>
   <si>
     <t>si</t>
@@ -248,7 +242,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +297,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -898,6 +898,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1580,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1619,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -1686,19 +1689,19 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="F2" s="16">
         <v>4</v>
@@ -1712,19 +1715,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F3" s="16">
         <v>5</v>
@@ -1732,19 +1735,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F4" s="16">
         <v>6</v>
@@ -1752,19 +1755,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F5" s="23">
         <v>8</v>
@@ -1772,19 +1775,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F6" s="23">
         <v>9</v>
@@ -1792,19 +1795,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F7" s="23">
         <v>11</v>
@@ -1812,19 +1815,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F8" s="23">
         <v>12</v>
@@ -1832,19 +1835,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F9" s="23">
         <v>13</v>
@@ -1853,19 +1856,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F10" s="23">
         <v>14</v>
@@ -1874,19 +1877,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="23">
         <v>15</v>
@@ -1895,19 +1898,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>60</v>
       </c>
       <c r="F12" s="23">
         <v>16</v>
@@ -1916,19 +1919,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="F13" s="14">
         <v>18</v>
@@ -1936,19 +1939,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="F14" s="14">
         <v>19</v>
@@ -1965,7 +1968,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -1987,10 +1990,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="35">
         <v>1</v>
@@ -2009,7 +2012,7 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>28</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>28</v>
@@ -2031,7 +2034,7 @@
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>28</v>
@@ -2042,7 +2045,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>28</v>
@@ -2053,7 +2056,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>28</v>
@@ -2064,7 +2067,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="27" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>28</v>
@@ -2090,7 +2093,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2120,8 +2123,8 @@
       <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>71</v>
+      <c r="B2" s="41" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>28</v>
@@ -2151,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>28</v>
@@ -2165,11 +2168,11 @@
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>59</v>
+      <c r="B5" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
@@ -2180,11 +2183,11 @@
       <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
@@ -2195,11 +2198,11 @@
       <c r="A7" s="19">
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
@@ -2211,7 +2214,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>28</v>
@@ -2225,11 +2228,11 @@
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>61</v>
+      <c r="B9" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
@@ -2240,11 +2243,11 @@
       <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>62</v>
+      <c r="B10" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -2256,7 +2259,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>28</v>
@@ -2270,11 +2273,11 @@
       <c r="A12" s="21">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>63</v>
+      <c r="B12" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2285,11 +2288,11 @@
       <c r="A13" s="21">
         <v>12</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>64</v>
+      <c r="B13" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2300,11 +2303,11 @@
       <c r="A14" s="21">
         <v>13</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>65</v>
+      <c r="B14" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -2315,11 +2318,11 @@
       <c r="A15" s="21">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>66</v>
+      <c r="B15" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -2330,11 +2333,11 @@
       <c r="A16" s="21">
         <v>15</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -2345,11 +2348,11 @@
       <c r="A17" s="21">
         <v>16</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>67</v>
+      <c r="B17" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -2361,7 +2364,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>28</v>
@@ -2375,11 +2378,11 @@
       <c r="A19" s="25">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>68</v>
+      <c r="B19" s="25" t="s">
+        <v>66</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2390,11 +2393,11 @@
       <c r="A20" s="25">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>69</v>
+      <c r="B20" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -2406,7 +2409,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>28</v>
@@ -2421,7 +2424,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>28</v>
@@ -2472,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:I58"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
@@ -2523,10 +2526,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2540,14 +2543,14 @@
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -2559,14 +2562,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -2578,14 +2581,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2597,14 +2600,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2616,14 +2619,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -2635,14 +2638,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2654,14 +2657,14 @@
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -2673,14 +2676,14 @@
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2692,14 +2695,14 @@
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2711,14 +2714,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -2730,14 +2733,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -2749,14 +2752,14 @@
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
@@ -2768,14 +2771,14 @@
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -2787,14 +2790,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2806,14 +2809,14 @@
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2825,19 +2828,19 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>28</v>
@@ -2848,14 +2851,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2867,14 +2870,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2886,14 +2889,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -2909,14 +2912,14 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2928,19 +2931,19 @@
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>28</v>
@@ -2951,10 +2954,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -2968,10 +2971,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2985,10 +2988,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3002,20 +3005,20 @@
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -3023,10 +3026,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3036,7 +3039,7 @@
         <v>24</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -3044,10 +3047,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3057,7 +3060,7 @@
         <v>25</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -3065,14 +3068,14 @@
         <v>19</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -3084,19 +3087,19 @@
         <v>19</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>28</v>
@@ -3107,10 +3110,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -3124,20 +3127,20 @@
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
@@ -3145,14 +3148,14 @@
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3164,22 +3167,22 @@
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
@@ -3187,18 +3190,18 @@
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -3208,18 +3211,18 @@
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -3229,18 +3232,18 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -3250,18 +3253,18 @@
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -3271,18 +3274,18 @@
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -3292,21 +3295,21 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I41" s="22" t="s">
         <v>28</v>
@@ -3317,18 +3320,18 @@
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
@@ -3338,18 +3341,18 @@
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
@@ -3359,18 +3362,18 @@
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
@@ -3380,18 +3383,18 @@
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
@@ -3401,24 +3404,24 @@
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -3426,24 +3429,24 @@
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -3451,24 +3454,24 @@
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -3476,14 +3479,14 @@
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
@@ -3495,22 +3498,22 @@
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -3518,14 +3521,14 @@
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
@@ -3533,7 +3536,7 @@
         <v>26</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
@@ -3541,22 +3544,22 @@
         <v>19</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -3564,14 +3567,14 @@
         <v>19</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
@@ -3583,19 +3586,19 @@
         <v>19</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I54" s="22" t="s">
         <v>28</v>
@@ -3606,20 +3609,20 @@
         <v>19</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
       <c r="H55" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -3627,20 +3630,20 @@
         <v>19</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
       <c r="G56" s="26"/>
       <c r="H56" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -3648,10 +3651,10 @@
         <v>19</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D57" s="40"/>
       <c r="E57" s="40"/>
@@ -3667,17 +3670,17 @@
         <v>19</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
       <c r="G58" s="40"/>
       <c r="H58" s="40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I58" s="40" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Ajuste nombre autoevaluación por evaluación
Ajuste nombre autoevaluación por evaluación tanto en guion como en
esqueleto de guion.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="106" yWindow="2774" windowWidth="15109" windowHeight="5971" tabRatio="729"/>
+    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1583,17 +1583,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="2" max="2" width="136.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="136.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1651,23 +1651,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>55</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>55</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>55</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>55</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>55</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>55</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>55</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>55</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>55</v>
       </c>
@@ -1875,7 +1875,7 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>55</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>55</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>55</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>55</v>
       </c>
@@ -1971,13 +1971,13 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.3984375" customWidth="1"/>
-    <col min="2" max="2" width="14.73046875" customWidth="1"/>
+    <col min="1" max="1" width="76.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>69</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>53</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>30</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>31</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
         <v>32</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
         <v>52</v>
       </c>
@@ -2092,19 +2092,19 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.59765625" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <v>1</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="G3" s="38"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2164,7 +2164,7 @@
       <c r="G4" s="39"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>4</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="G5" s="39"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>5</v>
       </c>
@@ -2194,7 +2194,7 @@
       <c r="G6" s="39"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>6</v>
       </c>
@@ -2209,7 +2209,7 @@
       <c r="G7" s="39"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>7</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="G8" s="39"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -2239,7 +2239,7 @@
       <c r="G9" s="39"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -2254,7 +2254,7 @@
       <c r="G10" s="39"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -2284,7 +2284,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -2299,7 +2299,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>16</v>
       </c>
@@ -2359,7 +2359,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -2374,7 +2374,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>18</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>19</v>
       </c>
@@ -2404,7 +2404,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <v>20</v>
       </c>
@@ -2419,7 +2419,7 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <v>21</v>
       </c>
@@ -2434,31 +2434,31 @@
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
     </row>
   </sheetData>
@@ -2475,24 +2475,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="D30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="1"/>
-    <col min="2" max="2" width="70.1328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.73046875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="47.73046875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.73046875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="71.59765625" customWidth="1"/>
-    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="71.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
@@ -2576,7 +2576,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>19</v>
       </c>
@@ -2595,7 +2595,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
@@ -2614,7 +2614,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>19</v>
       </c>
@@ -2633,7 +2633,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
@@ -2652,7 +2652,7 @@
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
@@ -2671,7 +2671,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>19</v>
       </c>
@@ -2690,7 +2690,7 @@
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
@@ -2709,7 +2709,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -2728,7 +2728,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>19</v>
       </c>
@@ -2766,7 +2766,7 @@
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>19</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>19</v>
       </c>
@@ -2804,7 +2804,7 @@
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>19</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>19</v>
       </c>
@@ -2865,7 +2865,7 @@
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
@@ -2884,7 +2884,7 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>19</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>19</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>19</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
@@ -2983,7 +2983,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>19</v>
       </c>
@@ -3000,7 +3000,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>19</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
         <v>19</v>
       </c>
@@ -3042,7 +3042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>19</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>19</v>
       </c>
@@ -3082,7 +3082,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>19</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>19</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="H32" s="23"/>
       <c r="I32" s="23"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
         <v>19</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>19</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
         <v>19</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
         <v>19</v>
       </c>
@@ -3206,7 +3206,7 @@
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>19</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>19</v>
       </c>
@@ -3248,7 +3248,7 @@
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>19</v>
       </c>
@@ -3269,7 +3269,7 @@
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>19</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>19</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>19</v>
       </c>
@@ -3336,7 +3336,7 @@
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>19</v>
       </c>
@@ -3357,7 +3357,7 @@
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>19</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>19</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
         <v>19</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
         <v>19</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>19</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
         <v>19</v>
       </c>
@@ -3493,7 +3493,7 @@
       <c r="H49" s="23"/>
       <c r="I49" s="23"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>19</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>19</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>19</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>19</v>
       </c>
@@ -3581,7 +3581,7 @@
       <c r="H53" s="23"/>
       <c r="I53" s="23"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
         <v>19</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
         <v>19</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>19</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
         <v>19</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
         <v>19</v>
       </c>
@@ -3686,19 +3686,19 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisión esqueleto de guion mat 7
Comprobación de nombres de recursos aprovechados
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1968,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,7 +2092,7 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="D30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revisión de esqueleto cuaderno de estudio mat 7 tema 1
Ajuste de títulos en manuscrito y guion mat 7 tema 1
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="71">
   <si>
     <t>FICHA</t>
   </si>
@@ -139,30 +139,18 @@
     <t>Foto</t>
   </si>
   <si>
-    <t>Números opuestos</t>
-  </si>
-  <si>
     <t>Recuerda</t>
   </si>
   <si>
-    <t>Definición de los números enteros</t>
-  </si>
-  <si>
     <t>Destacado</t>
   </si>
   <si>
     <t>Practica</t>
   </si>
   <si>
-    <t>Representación en la recta numérica de los números enteros</t>
-  </si>
-  <si>
     <t>Consolidación</t>
   </si>
   <si>
-    <t>Relaciones de orden en los números enteros</t>
-  </si>
-  <si>
     <t>¿Para qué sirven los números enteros?</t>
   </si>
   <si>
@@ -172,12 +160,6 @@
     <t>La aplicación de los números enteros en las matemáticas</t>
   </si>
   <si>
-    <t>Representación de puntos en el plano cartesiano</t>
-  </si>
-  <si>
-    <t>Valor absoluto</t>
-  </si>
-  <si>
     <t>La aplicación de los números enteros en la vida cotidiana</t>
   </si>
   <si>
@@ -235,7 +217,25 @@
     <t>Construcción de una recta numérica</t>
   </si>
   <si>
-    <t>Más información</t>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>La definición de los números enteros</t>
+  </si>
+  <si>
+    <t>Los números opuestos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La representación de los números enteros en la recta numérica </t>
+  </si>
+  <si>
+    <t>Las relaciones de orden en los números enteros</t>
+  </si>
+  <si>
+    <t>La representación de puntos en el plano cartesiano</t>
+  </si>
+  <si>
+    <t>El valor absoluto</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1689,19 +1689,19 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F2" s="16">
         <v>4</v>
@@ -1715,19 +1715,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F3" s="16">
         <v>5</v>
@@ -1735,19 +1735,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F4" s="16">
         <v>6</v>
@@ -1755,19 +1755,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F5" s="23">
         <v>8</v>
@@ -1775,19 +1775,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F6" s="23">
         <v>9</v>
@@ -1795,19 +1795,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F7" s="23">
         <v>11</v>
@@ -1815,19 +1815,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>62</v>
-      </c>
       <c r="E8" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F8" s="23">
         <v>12</v>
@@ -1835,19 +1835,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F9" s="23">
         <v>13</v>
@@ -1856,19 +1856,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F10" s="23">
         <v>14</v>
@@ -1877,19 +1877,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F11" s="23">
         <v>15</v>
@@ -1898,19 +1898,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F12" s="23">
         <v>16</v>
@@ -1919,19 +1919,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F13" s="14">
         <v>18</v>
@@ -1939,19 +1939,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F14" s="14">
         <v>19</v>
@@ -1990,7 +1990,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>33</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>28</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>28</v>
@@ -2124,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>28</v>
@@ -2154,7 +2154,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>28</v>
@@ -2169,7 +2169,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>33</v>
@@ -2229,7 +2229,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>33</v>
@@ -2244,7 +2244,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>33</v>
@@ -2274,7 +2274,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>33</v>
@@ -2289,7 +2289,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" s="30" t="s">
         <v>33</v>
@@ -2304,7 +2304,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>33</v>
@@ -2319,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>33</v>
@@ -2349,7 +2349,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>33</v>
@@ -2379,7 +2379,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>33</v>
@@ -2394,7 +2394,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>33</v>
@@ -2424,7 +2424,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>28</v>
@@ -2473,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,7 +2604,7 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>34</v>
@@ -2623,10 +2623,10 @@
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -2642,10 +2642,10 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>34</v>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>37</v>
@@ -2699,10 +2699,10 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>34</v>
@@ -2737,10 +2737,10 @@
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>34</v>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>34</v>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>37</v>
@@ -2813,10 +2813,10 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2832,15 +2832,15 @@
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>43</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="34" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>28</v>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>34</v>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>37</v>
@@ -2893,10 +2893,10 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>34</v>
@@ -2935,15 +2935,15 @@
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I23" s="17" t="s">
         <v>28</v>
@@ -2954,7 +2954,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>34</v>
@@ -2971,7 +2971,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>37</v>
@@ -2988,10 +2988,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3005,17 +3005,17 @@
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>33</v>
@@ -3026,10 +3026,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3047,10 +3047,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3068,11 +3068,11 @@
         <v>19</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>34</v>
@@ -3087,14 +3087,14 @@
         <v>19</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
@@ -3110,7 +3110,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>34</v>
@@ -3127,17 +3127,17 @@
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I33" s="23" t="s">
         <v>33</v>
@@ -3148,11 +3148,11 @@
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>34</v>
@@ -3167,19 +3167,19 @@
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I35" s="22" t="s">
         <v>33</v>
@@ -3190,15 +3190,15 @@
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G36" s="22" t="s">
         <v>34</v>
@@ -3211,15 +3211,15 @@
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G37" s="22" t="s">
         <v>37</v>
@@ -3232,18 +3232,18 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -3253,15 +3253,15 @@
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>37</v>
@@ -3274,15 +3274,15 @@
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G40" s="22" t="s">
         <v>34</v>
@@ -3295,18 +3295,18 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H41" s="21" t="s">
         <v>30</v>
@@ -3320,15 +3320,15 @@
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>34</v>
@@ -3341,15 +3341,15 @@
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G43" s="22" t="s">
         <v>37</v>
@@ -3362,18 +3362,18 @@
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
@@ -3383,15 +3383,15 @@
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>34</v>
@@ -3404,21 +3404,21 @@
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I46" s="22" t="s">
         <v>33</v>
@@ -3429,21 +3429,21 @@
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I47" s="22" t="s">
         <v>33</v>
@@ -3454,21 +3454,21 @@
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="21" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I48" s="22" t="s">
         <v>33</v>
@@ -3479,11 +3479,11 @@
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E49" s="22" t="s">
         <v>34</v>
@@ -3498,19 +3498,19 @@
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I50" s="22" t="s">
         <v>33</v>
@@ -3521,14 +3521,14 @@
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
@@ -3544,19 +3544,19 @@
         <v>19</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I52" s="22" t="s">
         <v>33</v>
@@ -3567,11 +3567,11 @@
         <v>19</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E53" s="22" t="s">
         <v>34</v>
@@ -3586,14 +3586,14 @@
         <v>19</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
@@ -3609,60 +3609,58 @@
         <v>19</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
       <c r="G55" s="26"/>
-      <c r="H55" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I55" s="26" t="s">
-        <v>33</v>
-      </c>
+      <c r="H55" s="14"/>
+      <c r="I55" s="26"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
       <c r="G56" s="26"/>
       <c r="H56" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I56" s="26" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40" t="s">
-        <v>28</v>
+      <c r="A57" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" s="26" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3670,24 +3668,40 @@
         <v>19</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
       <c r="F58" s="40"/>
       <c r="G58" s="40"/>
-      <c r="H58" s="40" t="s">
-        <v>52</v>
-      </c>
+      <c r="H58" s="40"/>
       <c r="I58" s="40" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+      <c r="A59" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="I59" s="40" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -3700,6 +3714,9 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajuste solicitado por Pedro Ortiz
Se encontraron dos recursos con el mismo contenido, se ajustó el error,
el recurso estaba mal nombrado. Se hicieron los ajustes y agregó el
contenido del recurso que debía estar en su lugar.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/esqueletoGuion_MA_07_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="105" yWindow="2775" windowWidth="15105" windowHeight="5970" tabRatio="729" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>¿Qué sabes de los números enteros?</t>
   </si>
   <si>
-    <t>¿Cómo hacer una recta numérica?</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>El valor absoluto</t>
+  </si>
+  <si>
+    <t>Ubicación de números enteros en la recta numérica</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1689,19 +1689,19 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>52</v>
       </c>
       <c r="F2" s="16">
         <v>4</v>
@@ -1715,19 +1715,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="16">
         <v>5</v>
@@ -1735,19 +1735,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="16">
         <v>6</v>
@@ -1755,19 +1755,19 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="23">
         <v>8</v>
@@ -1775,19 +1775,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="23">
         <v>9</v>
@@ -1795,19 +1795,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="23">
         <v>11</v>
@@ -1815,19 +1815,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="23">
         <v>12</v>
@@ -1835,19 +1835,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="23">
         <v>13</v>
@@ -1856,19 +1856,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="23">
         <v>14</v>
@@ -1877,19 +1877,19 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="23">
         <v>15</v>
@@ -1898,19 +1898,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="23">
         <v>16</v>
@@ -1919,19 +1919,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="14">
         <v>18</v>
@@ -1939,19 +1939,19 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="14">
         <v>19</v>
@@ -1968,7 +1968,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="35">
         <v>1</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>28</v>
       </c>
       <c r="C3" s="15">
         <v>2</v>
@@ -2012,10 +2012,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="15">
         <v>3</v>
@@ -2023,10 +2023,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="19">
         <v>7</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="33">
         <v>10</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="33">
         <v>17</v>
@@ -2056,10 +2056,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="27">
         <v>20</v>
@@ -2067,10 +2067,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="27">
         <v>21</v>
@@ -2093,7 +2093,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,10 +2124,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2139,10 +2139,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>28</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
@@ -2154,10 +2154,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
@@ -2169,10 +2169,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
@@ -2187,7 +2187,7 @@
         <v>24</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
@@ -2202,7 +2202,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
@@ -2214,10 +2214,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="39"/>
       <c r="F8" s="39"/>
@@ -2229,10 +2229,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
@@ -2244,10 +2244,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
@@ -2259,10 +2259,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -2274,10 +2274,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -2289,10 +2289,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -2304,10 +2304,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -2319,10 +2319,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -2337,7 +2337,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -2349,10 +2349,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -2364,10 +2364,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -2379,10 +2379,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -2394,10 +2394,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -2409,10 +2409,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -2424,10 +2424,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -2475,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,10 +2526,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
@@ -2543,14 +2543,14 @@
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
@@ -2562,14 +2562,14 @@
         <v>19</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -2581,14 +2581,14 @@
         <v>19</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -2600,14 +2600,14 @@
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -2619,14 +2619,14 @@
         <v>19</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -2638,14 +2638,14 @@
         <v>19</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2657,14 +2657,14 @@
         <v>19</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -2676,14 +2676,14 @@
         <v>19</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2695,14 +2695,14 @@
         <v>19</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2714,14 +2714,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -2733,14 +2733,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
@@ -2752,14 +2752,14 @@
         <v>19</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
@@ -2771,14 +2771,14 @@
         <v>19</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -2790,14 +2790,14 @@
         <v>19</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2809,14 +2809,14 @@
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2828,22 +2828,22 @@
         <v>19</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2851,14 +2851,14 @@
         <v>19</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2870,14 +2870,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2889,22 +2889,22 @@
         <v>19</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2912,14 +2912,14 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2931,22 +2931,22 @@
         <v>19</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2954,10 +2954,10 @@
         <v>19</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -2971,10 +2971,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
@@ -2988,10 +2988,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
@@ -3005,20 +3005,20 @@
         <v>19</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3026,10 +3026,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3039,7 +3039,7 @@
         <v>24</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3047,10 +3047,10 @@
         <v>19</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -3060,7 +3060,7 @@
         <v>25</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3068,14 +3068,14 @@
         <v>19</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -3087,22 +3087,22 @@
         <v>19</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
       <c r="H31" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3110,10 +3110,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -3127,20 +3127,20 @@
         <v>19</v>
       </c>
       <c r="B33" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>43</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
       <c r="H33" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,14 +3148,14 @@
         <v>19</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
@@ -3167,22 +3167,22 @@
         <v>19</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
       <c r="H35" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3190,18 +3190,18 @@
         <v>19</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
@@ -3211,18 +3211,18 @@
         <v>19</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -3232,18 +3232,18 @@
         <v>19</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="21"/>
       <c r="D38" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="23"/>
@@ -3253,18 +3253,18 @@
         <v>19</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" s="21"/>
       <c r="D39" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H39" s="23"/>
       <c r="I39" s="23"/>
@@ -3274,18 +3274,18 @@
         <v>19</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="21"/>
       <c r="D40" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H40" s="23"/>
       <c r="I40" s="23"/>
@@ -3295,24 +3295,24 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41" s="21"/>
       <c r="D41" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3320,18 +3320,18 @@
         <v>19</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" s="21"/>
       <c r="D42" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E42" s="22"/>
       <c r="F42" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G42" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H42" s="23"/>
       <c r="I42" s="23"/>
@@ -3341,18 +3341,18 @@
         <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43" s="22"/>
       <c r="F43" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H43" s="23"/>
       <c r="I43" s="23"/>
@@ -3362,18 +3362,18 @@
         <v>19</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" s="21"/>
       <c r="D44" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E44" s="22"/>
       <c r="F44" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G44" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23"/>
@@ -3383,18 +3383,18 @@
         <v>19</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="21"/>
       <c r="D45" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
@@ -3404,24 +3404,24 @@
         <v>19</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G46" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H46" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3429,24 +3429,24 @@
         <v>19</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H47" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3454,24 +3454,24 @@
         <v>19</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" s="21"/>
       <c r="D48" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E48" s="22"/>
       <c r="F48" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3479,14 +3479,14 @@
         <v>19</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F49" s="22"/>
       <c r="G49" s="22"/>
@@ -3498,22 +3498,22 @@
         <v>19</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F50" s="22"/>
       <c r="G50" s="22"/>
       <c r="H50" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3521,14 +3521,14 @@
         <v>19</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C51" s="21"/>
       <c r="D51" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F51" s="22"/>
       <c r="G51" s="22"/>
@@ -3536,7 +3536,7 @@
         <v>26</v>
       </c>
       <c r="I51" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3544,22 +3544,22 @@
         <v>19</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E52" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F52" s="22"/>
       <c r="G52" s="22"/>
       <c r="H52" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3567,14 +3567,14 @@
         <v>19</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
@@ -3586,22 +3586,22 @@
         <v>19</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F54" s="22"/>
       <c r="G54" s="22"/>
       <c r="H54" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3609,10 +3609,10 @@
         <v>19</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
@@ -3626,20 +3626,20 @@
         <v>19</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
       <c r="G56" s="26"/>
       <c r="H56" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I56" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,20 +3647,20 @@
         <v>19</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
       <c r="G57" s="26"/>
       <c r="H57" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I57" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3668,10 +3668,10 @@
         <v>19</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
@@ -3679,7 +3679,7 @@
       <c r="G58" s="40"/>
       <c r="H58" s="40"/>
       <c r="I58" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3687,20 +3687,20 @@
         <v>19</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D59" s="40"/>
       <c r="E59" s="40"/>
       <c r="F59" s="40"/>
       <c r="G59" s="40"/>
       <c r="H59" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I59" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>